<commit_message>
A_scrape_homegate.py updated, path for file creation changed.
</commit_message>
<xml_diff>
--- a/Data/results/results_supplementary_question.xlsx
+++ b/Data/results/results_supplementary_question.xlsx
@@ -513,460 +513,460 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2560</t>
+          <t>2502</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Nidau</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>31</v>
+        <v>200</v>
       </c>
       <c r="D2" t="n">
-        <v>17.85</v>
+        <v>140.97</v>
       </c>
       <c r="E2" t="n">
-        <v>-18.28</v>
+        <v>-80.87</v>
       </c>
       <c r="F2" t="n">
-        <v>5.66</v>
+        <v>110.95</v>
       </c>
       <c r="G2" t="n">
-        <v>-8.58</v>
+        <v>73.77</v>
       </c>
       <c r="H2" t="n">
-        <v>204.49</v>
+        <v>212.16</v>
       </c>
       <c r="I2" t="n">
-        <v>-232.04</v>
+        <v>304.91</v>
       </c>
       <c r="J2" t="n">
-        <v>12.96</v>
+        <v>-41.03</v>
       </c>
       <c r="K2" t="n">
-        <v>337.86</v>
+        <v>121.69</v>
       </c>
       <c r="L2" t="n">
-        <v>70.78</v>
+        <v>-73.78</v>
       </c>
       <c r="M2" t="n">
-        <v>-102.03</v>
+        <v>66.14</v>
       </c>
       <c r="N2" t="n">
-        <v>-78.64</v>
+        <v>-85.2</v>
       </c>
       <c r="O2" t="n">
-        <v>-0</v>
+        <v>-370.56</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2503</t>
+          <t>4912</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Aarwangen</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>170</v>
+        <v>26</v>
       </c>
       <c r="D3" t="n">
-        <v>45.56</v>
+        <v>71.78</v>
       </c>
       <c r="E3" t="n">
-        <v>34.85</v>
+        <v>280.38</v>
       </c>
       <c r="F3" t="n">
-        <v>82.02</v>
+        <v>354.29</v>
       </c>
       <c r="G3" t="n">
-        <v>-48.1</v>
+        <v>-125.02</v>
       </c>
       <c r="H3" t="n">
-        <v>211.98</v>
+        <v>513.88</v>
       </c>
       <c r="I3" t="n">
-        <v>391.57</v>
+        <v>393.41</v>
       </c>
       <c r="J3" t="n">
-        <v>244.93</v>
+        <v>-0</v>
       </c>
       <c r="K3" t="n">
-        <v>79.42</v>
+        <v>-18.33</v>
       </c>
       <c r="L3" t="n">
-        <v>-46.71</v>
+        <v>-98</v>
       </c>
       <c r="M3" t="n">
-        <v>-2.64</v>
+        <v>-8.74</v>
       </c>
       <c r="N3" t="n">
-        <v>59.75</v>
+        <v>-40.79</v>
       </c>
       <c r="O3" t="n">
-        <v>56.46</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4922</t>
+          <t>3014</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bützberg</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="D4" t="n">
-        <v>-27.36</v>
+        <v>122.62</v>
       </c>
       <c r="E4" t="n">
-        <v>161.33</v>
+        <v>-17.98</v>
       </c>
       <c r="F4" t="n">
-        <v>412.9</v>
+        <v>98.73</v>
       </c>
       <c r="G4" t="n">
-        <v>-266.33</v>
+        <v>-180.25</v>
       </c>
       <c r="H4" t="n">
-        <v>108.88</v>
+        <v>-0</v>
       </c>
       <c r="I4" t="n">
-        <v>-0</v>
+        <v>932.66</v>
       </c>
       <c r="J4" t="n">
-        <v>-0</v>
+        <v>427.22</v>
       </c>
       <c r="K4" t="n">
-        <v>306.15</v>
+        <v>285.62</v>
       </c>
       <c r="L4" t="n">
-        <v>196.01</v>
+        <v>61.28</v>
       </c>
       <c r="M4" t="n">
-        <v>109.56</v>
+        <v>0.46</v>
       </c>
       <c r="N4" t="n">
-        <v>237.57</v>
+        <v>-169.01</v>
       </c>
       <c r="O4" t="n">
-        <v>165.34</v>
+        <v>-128.79</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>3400</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Burgdorf</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D5" t="n">
-        <v>122.62</v>
+        <v>-16.99</v>
       </c>
       <c r="E5" t="n">
-        <v>-17.98</v>
+        <v>126.14</v>
       </c>
       <c r="F5" t="n">
-        <v>98.73</v>
+        <v>57</v>
       </c>
       <c r="G5" t="n">
-        <v>-180.25</v>
+        <v>138.78</v>
       </c>
       <c r="H5" t="n">
-        <v>-0</v>
+        <v>206.61</v>
       </c>
       <c r="I5" t="n">
-        <v>932.66</v>
+        <v>-0</v>
       </c>
       <c r="J5" t="n">
-        <v>427.22</v>
+        <v>246.1</v>
       </c>
       <c r="K5" t="n">
-        <v>285.62</v>
+        <v>223.49</v>
       </c>
       <c r="L5" t="n">
-        <v>61.28</v>
+        <v>146.57</v>
       </c>
       <c r="M5" t="n">
-        <v>0.46</v>
+        <v>-285.68</v>
       </c>
       <c r="N5" t="n">
-        <v>-169.01</v>
+        <v>-4.57</v>
       </c>
       <c r="O5" t="n">
-        <v>-128.79</v>
+        <v>-3.99</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3414</t>
+          <t>3008</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Oberburg</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="D6" t="n">
-        <v>15.37</v>
+        <v>-437.15</v>
       </c>
       <c r="E6" t="n">
+        <v>393.76</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-9.85</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-90.37</v>
+      </c>
+      <c r="H6" t="n">
+        <v>352.94</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-89.97</v>
+      </c>
+      <c r="J6" t="n">
+        <v>205.93</v>
+      </c>
+      <c r="K6" t="n">
+        <v>75.23</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-123.67</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-38.08</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-160.54</v>
+      </c>
+      <c r="O6" t="n">
         <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>233.14</v>
-      </c>
-      <c r="G6" t="n">
-        <v>284.46</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>-527.28</v>
-      </c>
-      <c r="J6" t="n">
-        <v>349.82</v>
-      </c>
-      <c r="K6" t="n">
-        <v>-527.28</v>
-      </c>
-      <c r="L6" t="n">
-        <v>-590.77</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-      <c r="N6" t="n">
-        <v>353.43</v>
-      </c>
-      <c r="O6" t="n">
-        <v>-590.77</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2502</t>
+          <t>3322</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Urtenen-Schönbühl</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>200</v>
+        <v>24</v>
       </c>
       <c r="D7" t="n">
-        <v>140.97</v>
+        <v>-72.22</v>
       </c>
       <c r="E7" t="n">
-        <v>-80.87</v>
+        <v>114.24</v>
       </c>
       <c r="F7" t="n">
-        <v>110.95</v>
+        <v>24.27</v>
       </c>
       <c r="G7" t="n">
-        <v>73.77</v>
+        <v>-119.38</v>
       </c>
       <c r="H7" t="n">
-        <v>212.16</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
-        <v>304.91</v>
+        <v>28.17</v>
       </c>
       <c r="J7" t="n">
-        <v>-41.03</v>
+        <v>53.19</v>
       </c>
       <c r="K7" t="n">
-        <v>121.69</v>
+        <v>-25.73</v>
       </c>
       <c r="L7" t="n">
-        <v>-73.78</v>
+        <v>85.84</v>
       </c>
       <c r="M7" t="n">
-        <v>66.14</v>
+        <v>-152.09</v>
       </c>
       <c r="N7" t="n">
-        <v>-85.2</v>
+        <v>60.13</v>
       </c>
       <c r="O7" t="n">
-        <v>-370.56</v>
+        <v>52.04</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4914</t>
+          <t>3414</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Roggwil BE</t>
+          <t>Oberburg</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D8" t="n">
-        <v>-65.79000000000001</v>
+        <v>15.37</v>
       </c>
       <c r="E8" t="n">
-        <v>134.94</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>-60.78</v>
+        <v>233.14</v>
       </c>
       <c r="G8" t="n">
-        <v>103</v>
+        <v>284.46</v>
       </c>
       <c r="H8" t="n">
-        <v>-83.68000000000001</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>-527.28</v>
       </c>
       <c r="J8" t="n">
-        <v>73.14</v>
+        <v>349.82</v>
       </c>
       <c r="K8" t="n">
-        <v>-95.22</v>
+        <v>-527.28</v>
       </c>
       <c r="L8" t="n">
-        <v>-26.73</v>
+        <v>-590.77</v>
       </c>
       <c r="M8" t="n">
         <v>0</v>
       </c>
       <c r="N8" t="n">
-        <v>-1.22</v>
+        <v>353.43</v>
       </c>
       <c r="O8" t="n">
-        <v>0</v>
+        <v>-590.77</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2504</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Thun</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>76</v>
+        <v>24</v>
       </c>
       <c r="D9" t="n">
-        <v>-15.72</v>
+        <v>207.02</v>
       </c>
       <c r="E9" t="n">
-        <v>55.74</v>
+        <v>252.93</v>
       </c>
       <c r="F9" t="n">
-        <v>-54.3</v>
+        <v>154.12</v>
       </c>
       <c r="G9" t="n">
-        <v>-97.48999999999999</v>
+        <v>-202.6</v>
       </c>
       <c r="H9" t="n">
-        <v>-0</v>
+        <v>205.69</v>
       </c>
       <c r="I9" t="n">
-        <v>37.13</v>
+        <v>-75.93000000000001</v>
       </c>
       <c r="J9" t="n">
-        <v>-44.7</v>
+        <v>424.62</v>
       </c>
       <c r="K9" t="n">
-        <v>272.76</v>
+        <v>159.97</v>
       </c>
       <c r="L9" t="n">
-        <v>42.35</v>
+        <v>399.38</v>
       </c>
       <c r="M9" t="n">
-        <v>-47.58</v>
+        <v>-36.73</v>
       </c>
       <c r="N9" t="n">
-        <v>-96.93000000000001</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="O9" t="n">
-        <v>-98.81</v>
+        <v>-309.26</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3027</t>
+          <t>3098</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Köniz</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D10" t="n">
-        <v>220.42</v>
+        <v>-79.42</v>
       </c>
       <c r="E10" t="n">
-        <v>284.87</v>
+        <v>67.02</v>
       </c>
       <c r="F10" t="n">
-        <v>195.56</v>
+        <v>49.57</v>
       </c>
       <c r="G10" t="n">
-        <v>274.62</v>
+        <v>-33.85</v>
       </c>
       <c r="H10" t="n">
-        <v>293.3</v>
+        <v>252.54</v>
       </c>
       <c r="I10" t="n">
-        <v>286.67</v>
+        <v>483.86</v>
       </c>
       <c r="J10" t="n">
-        <v>567.71</v>
+        <v>-0</v>
       </c>
       <c r="K10" t="n">
-        <v>155.65</v>
+        <v>314.85</v>
       </c>
       <c r="L10" t="n">
-        <v>-416.05</v>
+        <v>-16.51</v>
       </c>
       <c r="M10" t="n">
-        <v>-153.66</v>
+        <v>-17.51</v>
       </c>
       <c r="N10" t="n">
-        <v>78.76000000000001</v>
+        <v>-38.6</v>
       </c>
       <c r="O10" t="n">
-        <v>0</v>
+        <v>155.63</v>
       </c>
     </row>
     <row r="11">
@@ -1023,100 +1023,100 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3302</t>
+          <t>3013</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Moosseedorf</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="D12" t="n">
-        <v>-46.21</v>
+        <v>-66.02</v>
       </c>
       <c r="E12" t="n">
-        <v>114.91</v>
+        <v>-81.20999999999999</v>
       </c>
       <c r="F12" t="n">
-        <v>178.14</v>
+        <v>-84.18000000000001</v>
       </c>
       <c r="G12" t="n">
-        <v>-356.93</v>
+        <v>228.05</v>
       </c>
       <c r="H12" t="n">
-        <v>-358.43</v>
+        <v>109.6</v>
       </c>
       <c r="I12" t="n">
         <v>-0</v>
       </c>
       <c r="J12" t="n">
-        <v>279.22</v>
+        <v>-102.41</v>
       </c>
       <c r="K12" t="n">
-        <v>-10.83</v>
+        <v>327.77</v>
       </c>
       <c r="L12" t="n">
-        <v>-73.12</v>
+        <v>181.8</v>
       </c>
       <c r="M12" t="n">
-        <v>128.33</v>
+        <v>-252.55</v>
       </c>
       <c r="N12" t="n">
-        <v>53.29</v>
+        <v>61.62</v>
       </c>
       <c r="O12" t="n">
-        <v>-341.09</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>3097</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Liebefeld</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D13" t="n">
-        <v>-46.54</v>
+        <v>4.83</v>
       </c>
       <c r="E13" t="n">
-        <v>52.29</v>
+        <v>317.67</v>
       </c>
       <c r="F13" t="n">
-        <v>158.67</v>
+        <v>-53.57</v>
       </c>
       <c r="G13" t="n">
-        <v>-100</v>
+        <v>268.25</v>
       </c>
       <c r="H13" t="n">
         <v>-0</v>
       </c>
       <c r="I13" t="n">
-        <v>54.94</v>
+        <v>-0</v>
       </c>
       <c r="J13" t="n">
         <v>-0</v>
       </c>
       <c r="K13" t="n">
-        <v>155.38</v>
+        <v>165.67</v>
       </c>
       <c r="L13" t="n">
-        <v>-0</v>
+        <v>293.8</v>
       </c>
       <c r="M13" t="n">
-        <v>-184.61</v>
+        <v>-171.75</v>
       </c>
       <c r="N13" t="n">
-        <v>-16.47</v>
+        <v>-185.21</v>
       </c>
       <c r="O13" t="n">
         <v>-0</v>
@@ -1125,406 +1125,406 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3360</t>
+          <t>2560</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Herzogenbuchsee</t>
+          <t>Nidau</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D14" t="n">
-        <v>17.23</v>
+        <v>17.85</v>
       </c>
       <c r="E14" t="n">
-        <v>42.79</v>
+        <v>-18.28</v>
       </c>
       <c r="F14" t="n">
-        <v>180.84</v>
+        <v>5.66</v>
       </c>
       <c r="G14" t="n">
-        <v>-84.84</v>
+        <v>-8.58</v>
       </c>
       <c r="H14" t="n">
-        <v>0</v>
+        <v>204.49</v>
       </c>
       <c r="I14" t="n">
-        <v>33.96</v>
+        <v>-232.04</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>12.96</v>
       </c>
       <c r="K14" t="n">
-        <v>78.56999999999999</v>
+        <v>337.86</v>
       </c>
       <c r="L14" t="n">
-        <v>82.8</v>
+        <v>70.78</v>
       </c>
       <c r="M14" t="n">
-        <v>62.8</v>
+        <v>-102.03</v>
       </c>
       <c r="N14" t="n">
-        <v>87.58</v>
+        <v>-78.64</v>
       </c>
       <c r="O14" t="n">
-        <v>245.97</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>3250</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Lyss</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="D15" t="n">
-        <v>-38.69</v>
+        <v>211.29</v>
       </c>
       <c r="E15" t="n">
-        <v>-5.92</v>
+        <v>-88.04000000000001</v>
       </c>
       <c r="F15" t="n">
-        <v>89.33</v>
+        <v>78.73</v>
       </c>
       <c r="G15" t="n">
-        <v>53.71</v>
+        <v>50.71</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>-16.53</v>
       </c>
       <c r="I15" t="n">
-        <v>-73.17</v>
+        <v>123.09</v>
       </c>
       <c r="J15" t="n">
-        <v>0</v>
+        <v>61.1</v>
       </c>
       <c r="K15" t="n">
-        <v>80.76000000000001</v>
+        <v>325.03</v>
       </c>
       <c r="L15" t="n">
-        <v>95.14</v>
+        <v>49.2</v>
       </c>
       <c r="M15" t="n">
-        <v>-98.7</v>
+        <v>11.76</v>
       </c>
       <c r="N15" t="n">
-        <v>-71.63</v>
+        <v>108.48</v>
       </c>
       <c r="O15" t="n">
-        <v>0</v>
+        <v>70.54000000000001</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3097</t>
+          <t>4950</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Liebefeld</t>
+          <t>Huttwil</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D16" t="n">
-        <v>4.83</v>
+        <v>67.13</v>
       </c>
       <c r="E16" t="n">
-        <v>317.67</v>
+        <v>32.17</v>
       </c>
       <c r="F16" t="n">
-        <v>-53.57</v>
+        <v>273.14</v>
       </c>
       <c r="G16" t="n">
-        <v>268.25</v>
+        <v>-61.28</v>
       </c>
       <c r="H16" t="n">
         <v>-0</v>
       </c>
       <c r="I16" t="n">
-        <v>-0</v>
+        <v>615.97</v>
       </c>
       <c r="J16" t="n">
         <v>-0</v>
       </c>
       <c r="K16" t="n">
-        <v>165.67</v>
+        <v>388.76</v>
       </c>
       <c r="L16" t="n">
-        <v>293.8</v>
+        <v>275.64</v>
       </c>
       <c r="M16" t="n">
-        <v>-171.75</v>
+        <v>-40.09</v>
       </c>
       <c r="N16" t="n">
-        <v>-185.21</v>
+        <v>-104.11</v>
       </c>
       <c r="O16" t="n">
-        <v>-0</v>
+        <v>13.91</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>3110</t>
+          <t>2503</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Münsingen</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="D17" t="n">
-        <v>26.34</v>
+        <v>45.56</v>
       </c>
       <c r="E17" t="n">
-        <v>-73.05</v>
+        <v>34.85</v>
       </c>
       <c r="F17" t="n">
-        <v>121.32</v>
+        <v>82.02</v>
       </c>
       <c r="G17" t="n">
-        <v>61.99</v>
+        <v>-48.1</v>
       </c>
       <c r="H17" t="n">
-        <v>-0</v>
+        <v>211.98</v>
       </c>
       <c r="I17" t="n">
-        <v>-0</v>
+        <v>391.57</v>
       </c>
       <c r="J17" t="n">
-        <v>-0</v>
+        <v>244.93</v>
       </c>
       <c r="K17" t="n">
-        <v>250.53</v>
+        <v>79.42</v>
       </c>
       <c r="L17" t="n">
-        <v>-251.01</v>
+        <v>-46.71</v>
       </c>
       <c r="M17" t="n">
-        <v>-237.49</v>
+        <v>-2.64</v>
       </c>
       <c r="N17" t="n">
-        <v>26.06</v>
+        <v>59.75</v>
       </c>
       <c r="O17" t="n">
-        <v>-0</v>
+        <v>56.46</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3400</t>
+          <t>3052</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Burgdorf</t>
+          <t>Zollikofen</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>55</v>
+        <v>29</v>
       </c>
       <c r="D18" t="n">
-        <v>-16.99</v>
+        <v>73.94</v>
       </c>
       <c r="E18" t="n">
-        <v>126.14</v>
+        <v>45.36</v>
       </c>
       <c r="F18" t="n">
-        <v>57</v>
+        <v>347.56</v>
       </c>
       <c r="G18" t="n">
-        <v>138.78</v>
+        <v>157.68</v>
       </c>
       <c r="H18" t="n">
-        <v>206.61</v>
+        <v>382.34</v>
       </c>
       <c r="I18" t="n">
-        <v>-0</v>
+        <v>488.02</v>
       </c>
       <c r="J18" t="n">
-        <v>246.1</v>
+        <v>457.62</v>
       </c>
       <c r="K18" t="n">
-        <v>223.49</v>
+        <v>456.47</v>
       </c>
       <c r="L18" t="n">
-        <v>146.57</v>
+        <v>135.73</v>
       </c>
       <c r="M18" t="n">
-        <v>-285.68</v>
+        <v>39.84</v>
       </c>
       <c r="N18" t="n">
-        <v>-4.57</v>
+        <v>-228.55</v>
       </c>
       <c r="O18" t="n">
-        <v>-3.99</v>
+        <v>-59.51</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2555</t>
+          <t>3302</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Brügg BE</t>
+          <t>Moosseedorf</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="D19" t="n">
-        <v>41.52</v>
+        <v>-46.21</v>
       </c>
       <c r="E19" t="n">
-        <v>-44.19</v>
+        <v>114.91</v>
       </c>
       <c r="F19" t="n">
-        <v>6.89</v>
+        <v>178.14</v>
       </c>
       <c r="G19" t="n">
-        <v>4.3</v>
+        <v>-356.93</v>
       </c>
       <c r="H19" t="n">
-        <v>-0</v>
+        <v>-358.43</v>
       </c>
       <c r="I19" t="n">
-        <v>-75.98999999999999</v>
+        <v>-0</v>
       </c>
       <c r="J19" t="n">
-        <v>222.7</v>
+        <v>279.22</v>
       </c>
       <c r="K19" t="n">
-        <v>222.7</v>
+        <v>-10.83</v>
       </c>
       <c r="L19" t="n">
-        <v>10.49</v>
+        <v>-73.12</v>
       </c>
       <c r="M19" t="n">
-        <v>-0</v>
+        <v>128.33</v>
       </c>
       <c r="N19" t="n">
-        <v>-22.58</v>
+        <v>53.29</v>
       </c>
       <c r="O19" t="n">
-        <v>-73.26000000000001</v>
+        <v>-341.09</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4950</t>
+          <t>3018</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Huttwil</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D20" t="n">
-        <v>67.13</v>
+        <v>-196.57</v>
       </c>
       <c r="E20" t="n">
-        <v>32.17</v>
+        <v>-140.72</v>
       </c>
       <c r="F20" t="n">
-        <v>273.14</v>
+        <v>42.27</v>
       </c>
       <c r="G20" t="n">
-        <v>-61.28</v>
+        <v>119.98</v>
       </c>
       <c r="H20" t="n">
-        <v>-0</v>
+        <v>92.04000000000001</v>
       </c>
       <c r="I20" t="n">
-        <v>615.97</v>
+        <v>102.11</v>
       </c>
       <c r="J20" t="n">
-        <v>-0</v>
+        <v>92.48999999999999</v>
       </c>
       <c r="K20" t="n">
-        <v>388.76</v>
+        <v>71.45</v>
       </c>
       <c r="L20" t="n">
-        <v>275.64</v>
+        <v>35.82</v>
       </c>
       <c r="M20" t="n">
-        <v>-40.09</v>
+        <v>-99.56</v>
       </c>
       <c r="N20" t="n">
-        <v>-104.11</v>
+        <v>-47.17</v>
       </c>
       <c r="O20" t="n">
-        <v>13.91</v>
+        <v>-355.07</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3012</t>
+          <t>3270</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Aarberg</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>58</v>
+        <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>165.82</v>
+        <v>791.75</v>
       </c>
       <c r="E21" t="n">
-        <v>150.2</v>
+        <v>531.97</v>
       </c>
       <c r="F21" t="n">
-        <v>-39.57</v>
+        <v>-379.6</v>
       </c>
       <c r="G21" t="n">
-        <v>26.88</v>
+        <v>234.25</v>
       </c>
       <c r="H21" t="n">
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>363.75</v>
+        <v>164.45</v>
       </c>
       <c r="J21" t="n">
-        <v>581.58</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>229.38</v>
+        <v>475.69</v>
       </c>
       <c r="L21" t="n">
-        <v>232.29</v>
+        <v>164.45</v>
       </c>
       <c r="M21" t="n">
-        <v>-68.38</v>
+        <v>164.45</v>
       </c>
       <c r="N21" t="n">
-        <v>-22.6</v>
+        <v>164.45</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -1533,763 +1533,763 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>3073</t>
+          <t>4914</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Gümligen</t>
+          <t>Roggwil BE</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D22" t="n">
-        <v>-88.77</v>
+        <v>-65.79000000000001</v>
       </c>
       <c r="E22" t="n">
-        <v>126.5</v>
+        <v>134.94</v>
       </c>
       <c r="F22" t="n">
-        <v>41.54</v>
+        <v>-60.78</v>
       </c>
       <c r="G22" t="n">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="H22" t="n">
-        <v>123.04</v>
+        <v>-83.68000000000001</v>
       </c>
       <c r="I22" t="n">
-        <v>126.72</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>126.72</v>
+        <v>73.14</v>
       </c>
       <c r="K22" t="n">
-        <v>160.98</v>
+        <v>-95.22</v>
       </c>
       <c r="L22" t="n">
-        <v>85.52</v>
+        <v>-26.73</v>
       </c>
       <c r="M22" t="n">
-        <v>-187.81</v>
+        <v>0</v>
       </c>
       <c r="N22" t="n">
-        <v>102.04</v>
+        <v>-1.22</v>
       </c>
       <c r="O22" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Zollikofen</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D23" t="n">
-        <v>73.94</v>
+        <v>-46.54</v>
       </c>
       <c r="E23" t="n">
-        <v>45.36</v>
+        <v>52.29</v>
       </c>
       <c r="F23" t="n">
-        <v>347.56</v>
+        <v>158.67</v>
       </c>
       <c r="G23" t="n">
-        <v>157.68</v>
+        <v>-100</v>
       </c>
       <c r="H23" t="n">
-        <v>382.34</v>
+        <v>-0</v>
       </c>
       <c r="I23" t="n">
-        <v>488.02</v>
+        <v>54.94</v>
       </c>
       <c r="J23" t="n">
-        <v>457.62</v>
+        <v>-0</v>
       </c>
       <c r="K23" t="n">
-        <v>456.47</v>
+        <v>155.38</v>
       </c>
       <c r="L23" t="n">
-        <v>135.73</v>
+        <v>-0</v>
       </c>
       <c r="M23" t="n">
-        <v>39.84</v>
+        <v>-184.61</v>
       </c>
       <c r="N23" t="n">
-        <v>-228.55</v>
+        <v>-16.47</v>
       </c>
       <c r="O23" t="n">
-        <v>-59.51</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4912</t>
+          <t>3012</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Aarwangen</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="D24" t="n">
-        <v>71.78</v>
+        <v>165.82</v>
       </c>
       <c r="E24" t="n">
-        <v>280.38</v>
+        <v>150.2</v>
       </c>
       <c r="F24" t="n">
-        <v>354.29</v>
+        <v>-39.57</v>
       </c>
       <c r="G24" t="n">
-        <v>-125.02</v>
+        <v>26.88</v>
       </c>
       <c r="H24" t="n">
-        <v>513.88</v>
+        <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>393.41</v>
+        <v>363.75</v>
       </c>
       <c r="J24" t="n">
-        <v>-0</v>
+        <v>581.58</v>
       </c>
       <c r="K24" t="n">
-        <v>-18.33</v>
+        <v>229.38</v>
       </c>
       <c r="L24" t="n">
-        <v>-98</v>
+        <v>232.29</v>
       </c>
       <c r="M24" t="n">
-        <v>-8.74</v>
+        <v>-68.38</v>
       </c>
       <c r="N24" t="n">
-        <v>-40.79</v>
+        <v>-22.6</v>
       </c>
       <c r="O24" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>3084</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Thun</t>
+          <t>Wabern</t>
         </is>
       </c>
       <c r="C25" t="n">
         <v>24</v>
       </c>
       <c r="D25" t="n">
-        <v>207.02</v>
+        <v>6.43</v>
       </c>
       <c r="E25" t="n">
-        <v>252.93</v>
+        <v>-11.5</v>
       </c>
       <c r="F25" t="n">
-        <v>154.12</v>
+        <v>-219.67</v>
       </c>
       <c r="G25" t="n">
-        <v>-202.6</v>
+        <v>-196.73</v>
       </c>
       <c r="H25" t="n">
-        <v>205.69</v>
+        <v>90.03</v>
       </c>
       <c r="I25" t="n">
+        <v>952.75</v>
+      </c>
+      <c r="J25" t="n">
+        <v>-0</v>
+      </c>
+      <c r="K25" t="n">
+        <v>104.41</v>
+      </c>
+      <c r="L25" t="n">
+        <v>28.27</v>
+      </c>
+      <c r="M25" t="n">
+        <v>128.82</v>
+      </c>
+      <c r="N25" t="n">
+        <v>292.5</v>
+      </c>
+      <c r="O25" t="n">
         <v>-75.93000000000001</v>
-      </c>
-      <c r="J25" t="n">
-        <v>424.62</v>
-      </c>
-      <c r="K25" t="n">
-        <v>159.97</v>
-      </c>
-      <c r="L25" t="n">
-        <v>399.38</v>
-      </c>
-      <c r="M25" t="n">
-        <v>-36.73</v>
-      </c>
-      <c r="N25" t="n">
-        <v>69.09999999999999</v>
-      </c>
-      <c r="O25" t="n">
-        <v>-309.26</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3018</t>
+          <t>3072</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Ostermundigen</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="D26" t="n">
-        <v>-196.57</v>
+        <v>-149.15</v>
       </c>
       <c r="E26" t="n">
-        <v>-140.72</v>
+        <v>9.59</v>
       </c>
       <c r="F26" t="n">
-        <v>42.27</v>
+        <v>86.14</v>
       </c>
       <c r="G26" t="n">
-        <v>119.98</v>
+        <v>-60.65</v>
       </c>
       <c r="H26" t="n">
-        <v>92.04000000000001</v>
+        <v>-273.53</v>
       </c>
       <c r="I26" t="n">
-        <v>102.11</v>
+        <v>75.65000000000001</v>
       </c>
       <c r="J26" t="n">
-        <v>92.48999999999999</v>
+        <v>433.65</v>
       </c>
       <c r="K26" t="n">
-        <v>71.45</v>
+        <v>89.5</v>
       </c>
       <c r="L26" t="n">
-        <v>35.82</v>
+        <v>39.7</v>
       </c>
       <c r="M26" t="n">
-        <v>-99.56</v>
+        <v>-128.77</v>
       </c>
       <c r="N26" t="n">
-        <v>-47.17</v>
+        <v>45.48</v>
       </c>
       <c r="O26" t="n">
-        <v>-355.07</v>
+        <v>-61.79</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>3063</t>
+          <t>2555</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Ittigen</t>
+          <t>Brügg BE</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D27" t="n">
-        <v>37.39</v>
+        <v>41.52</v>
       </c>
       <c r="E27" t="n">
-        <v>431.11</v>
+        <v>-44.19</v>
       </c>
       <c r="F27" t="n">
-        <v>-186.35</v>
+        <v>6.89</v>
       </c>
       <c r="G27" t="n">
-        <v>698.52</v>
+        <v>4.3</v>
       </c>
       <c r="H27" t="n">
-        <v>334.87</v>
+        <v>-0</v>
       </c>
       <c r="I27" t="n">
-        <v>276.35</v>
+        <v>-75.98999999999999</v>
       </c>
       <c r="J27" t="n">
-        <v>104.12</v>
+        <v>222.7</v>
       </c>
       <c r="K27" t="n">
-        <v>165.96</v>
+        <v>222.7</v>
       </c>
       <c r="L27" t="n">
-        <v>354.2</v>
+        <v>10.49</v>
       </c>
       <c r="M27" t="n">
-        <v>-186.29</v>
+        <v>-0</v>
       </c>
       <c r="N27" t="n">
-        <v>-130.26</v>
+        <v>-22.58</v>
       </c>
       <c r="O27" t="n">
-        <v>-13.12</v>
+        <v>-73.26000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3322</t>
+          <t>3007</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Urtenen-Schönbühl</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="D28" t="n">
-        <v>-72.22</v>
+        <v>-38.69</v>
       </c>
       <c r="E28" t="n">
-        <v>114.24</v>
+        <v>-5.92</v>
       </c>
       <c r="F28" t="n">
-        <v>24.27</v>
+        <v>89.33</v>
       </c>
       <c r="G28" t="n">
-        <v>-119.38</v>
+        <v>53.71</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>28.17</v>
+        <v>-73.17</v>
       </c>
       <c r="J28" t="n">
-        <v>53.19</v>
+        <v>0</v>
       </c>
       <c r="K28" t="n">
-        <v>-25.73</v>
+        <v>80.76000000000001</v>
       </c>
       <c r="L28" t="n">
-        <v>85.84</v>
+        <v>95.14</v>
       </c>
       <c r="M28" t="n">
-        <v>-152.09</v>
+        <v>-98.7</v>
       </c>
       <c r="N28" t="n">
-        <v>60.13</v>
+        <v>-71.63</v>
       </c>
       <c r="O28" t="n">
-        <v>52.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4900</t>
+          <t>3063</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Langenthal</t>
+          <t>Ittigen</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="D29" t="n">
-        <v>-70.77</v>
+        <v>37.39</v>
       </c>
       <c r="E29" t="n">
-        <v>33.06</v>
+        <v>431.11</v>
       </c>
       <c r="F29" t="n">
-        <v>136.11</v>
+        <v>-186.35</v>
       </c>
       <c r="G29" t="n">
-        <v>-93.63</v>
+        <v>698.52</v>
       </c>
       <c r="H29" t="n">
-        <v>344.24</v>
+        <v>334.87</v>
       </c>
       <c r="I29" t="n">
-        <v>-39.78</v>
+        <v>276.35</v>
       </c>
       <c r="J29" t="n">
-        <v>288.97</v>
+        <v>104.12</v>
       </c>
       <c r="K29" t="n">
-        <v>53.77</v>
+        <v>165.96</v>
       </c>
       <c r="L29" t="n">
-        <v>31.59</v>
+        <v>354.2</v>
       </c>
       <c r="M29" t="n">
-        <v>-26.52</v>
+        <v>-186.29</v>
       </c>
       <c r="N29" t="n">
-        <v>13.54</v>
+        <v>-130.26</v>
       </c>
       <c r="O29" t="n">
-        <v>33.17</v>
+        <v>-13.12</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3011</t>
+          <t>3360</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Herzogenbuchsee</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="D30" t="n">
-        <v>-22.4</v>
+        <v>17.23</v>
       </c>
       <c r="E30" t="n">
-        <v>207.57</v>
+        <v>42.79</v>
       </c>
       <c r="F30" t="n">
-        <v>280.52</v>
+        <v>180.84</v>
       </c>
       <c r="G30" t="n">
-        <v>222.39</v>
+        <v>-84.84</v>
       </c>
       <c r="H30" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="I30" t="n">
-        <v>-181.31</v>
+        <v>33.96</v>
       </c>
       <c r="J30" t="n">
-        <v>-361.86</v>
+        <v>0</v>
       </c>
       <c r="K30" t="n">
-        <v>86.22</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="L30" t="n">
-        <v>-17.78</v>
+        <v>82.8</v>
       </c>
       <c r="M30" t="n">
-        <v>2.18</v>
+        <v>62.8</v>
       </c>
       <c r="N30" t="n">
-        <v>15.83</v>
+        <v>87.58</v>
       </c>
       <c r="O30" t="n">
-        <v>-0</v>
+        <v>245.97</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3084</t>
+          <t>3027</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Wabern</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D31" t="n">
-        <v>6.43</v>
+        <v>220.42</v>
       </c>
       <c r="E31" t="n">
-        <v>-11.5</v>
+        <v>284.87</v>
       </c>
       <c r="F31" t="n">
-        <v>-219.67</v>
+        <v>195.56</v>
       </c>
       <c r="G31" t="n">
-        <v>-196.73</v>
+        <v>274.62</v>
       </c>
       <c r="H31" t="n">
-        <v>90.03</v>
+        <v>293.3</v>
       </c>
       <c r="I31" t="n">
-        <v>952.75</v>
+        <v>286.67</v>
       </c>
       <c r="J31" t="n">
-        <v>-0</v>
+        <v>567.71</v>
       </c>
       <c r="K31" t="n">
-        <v>104.41</v>
+        <v>155.65</v>
       </c>
       <c r="L31" t="n">
-        <v>28.27</v>
+        <v>-416.05</v>
       </c>
       <c r="M31" t="n">
-        <v>128.82</v>
+        <v>-153.66</v>
       </c>
       <c r="N31" t="n">
-        <v>292.5</v>
+        <v>78.76000000000001</v>
       </c>
       <c r="O31" t="n">
-        <v>-75.93000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3072</t>
+          <t>3073</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ostermundigen</t>
+          <t>Gümligen</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="D32" t="n">
-        <v>-149.15</v>
+        <v>-88.77</v>
       </c>
       <c r="E32" t="n">
-        <v>9.59</v>
+        <v>126.5</v>
       </c>
       <c r="F32" t="n">
-        <v>86.14</v>
+        <v>41.54</v>
       </c>
       <c r="G32" t="n">
-        <v>-60.65</v>
+        <v>135</v>
       </c>
       <c r="H32" t="n">
-        <v>-273.53</v>
+        <v>123.04</v>
       </c>
       <c r="I32" t="n">
-        <v>75.65000000000001</v>
+        <v>126.72</v>
       </c>
       <c r="J32" t="n">
-        <v>433.65</v>
+        <v>126.72</v>
       </c>
       <c r="K32" t="n">
-        <v>89.5</v>
+        <v>160.98</v>
       </c>
       <c r="L32" t="n">
-        <v>39.7</v>
+        <v>85.52</v>
       </c>
       <c r="M32" t="n">
-        <v>-128.77</v>
+        <v>-187.81</v>
       </c>
       <c r="N32" t="n">
-        <v>45.48</v>
+        <v>102.04</v>
       </c>
       <c r="O32" t="n">
-        <v>-61.79</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3250</t>
+          <t>3011</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Lyss</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>64</v>
       </c>
       <c r="D33" t="n">
-        <v>211.29</v>
+        <v>-22.4</v>
       </c>
       <c r="E33" t="n">
-        <v>-88.04000000000001</v>
+        <v>207.57</v>
       </c>
       <c r="F33" t="n">
-        <v>78.73</v>
+        <v>280.52</v>
       </c>
       <c r="G33" t="n">
-        <v>50.71</v>
+        <v>222.39</v>
       </c>
       <c r="H33" t="n">
-        <v>-16.53</v>
+        <v>-0</v>
       </c>
       <c r="I33" t="n">
-        <v>123.09</v>
+        <v>-181.31</v>
       </c>
       <c r="J33" t="n">
-        <v>61.1</v>
+        <v>-361.86</v>
       </c>
       <c r="K33" t="n">
-        <v>325.03</v>
+        <v>86.22</v>
       </c>
       <c r="L33" t="n">
-        <v>49.2</v>
+        <v>-17.78</v>
       </c>
       <c r="M33" t="n">
-        <v>11.76</v>
+        <v>2.18</v>
       </c>
       <c r="N33" t="n">
-        <v>108.48</v>
+        <v>15.83</v>
       </c>
       <c r="O33" t="n">
-        <v>70.54000000000001</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>3008</t>
+          <t>2504</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>46</v>
+        <v>76</v>
       </c>
       <c r="D34" t="n">
-        <v>-437.15</v>
+        <v>-15.72</v>
       </c>
       <c r="E34" t="n">
-        <v>393.76</v>
+        <v>55.74</v>
       </c>
       <c r="F34" t="n">
-        <v>-9.85</v>
+        <v>-54.3</v>
       </c>
       <c r="G34" t="n">
-        <v>-90.37</v>
+        <v>-97.48999999999999</v>
       </c>
       <c r="H34" t="n">
-        <v>352.94</v>
+        <v>-0</v>
       </c>
       <c r="I34" t="n">
-        <v>-89.97</v>
+        <v>37.13</v>
       </c>
       <c r="J34" t="n">
-        <v>205.93</v>
+        <v>-44.7</v>
       </c>
       <c r="K34" t="n">
-        <v>75.23</v>
+        <v>272.76</v>
       </c>
       <c r="L34" t="n">
-        <v>-123.67</v>
+        <v>42.35</v>
       </c>
       <c r="M34" t="n">
-        <v>-38.08</v>
+        <v>-47.58</v>
       </c>
       <c r="N34" t="n">
-        <v>-160.54</v>
+        <v>-96.93000000000001</v>
       </c>
       <c r="O34" t="n">
-        <v>0</v>
+        <v>-98.81</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>3098</t>
+          <t>4922</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Köniz</t>
+          <t>Bützberg</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D35" t="n">
-        <v>-79.42</v>
+        <v>-27.36</v>
       </c>
       <c r="E35" t="n">
-        <v>67.02</v>
+        <v>161.33</v>
       </c>
       <c r="F35" t="n">
-        <v>49.57</v>
+        <v>412.9</v>
       </c>
       <c r="G35" t="n">
-        <v>-33.85</v>
+        <v>-266.33</v>
       </c>
       <c r="H35" t="n">
-        <v>252.54</v>
+        <v>108.88</v>
       </c>
       <c r="I35" t="n">
-        <v>483.86</v>
+        <v>-0</v>
       </c>
       <c r="J35" t="n">
         <v>-0</v>
       </c>
       <c r="K35" t="n">
-        <v>314.85</v>
+        <v>306.15</v>
       </c>
       <c r="L35" t="n">
-        <v>-16.51</v>
+        <v>196.01</v>
       </c>
       <c r="M35" t="n">
-        <v>-17.51</v>
+        <v>109.56</v>
       </c>
       <c r="N35" t="n">
-        <v>-38.6</v>
+        <v>237.57</v>
       </c>
       <c r="O35" t="n">
-        <v>155.63</v>
+        <v>165.34</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3013</t>
+          <t>3110</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Münsingen</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D36" t="n">
-        <v>-66.02</v>
+        <v>26.34</v>
       </c>
       <c r="E36" t="n">
-        <v>-81.20999999999999</v>
+        <v>-73.05</v>
       </c>
       <c r="F36" t="n">
-        <v>-84.18000000000001</v>
+        <v>121.32</v>
       </c>
       <c r="G36" t="n">
-        <v>228.05</v>
+        <v>61.99</v>
       </c>
       <c r="H36" t="n">
-        <v>109.6</v>
+        <v>-0</v>
       </c>
       <c r="I36" t="n">
         <v>-0</v>
       </c>
       <c r="J36" t="n">
-        <v>-102.41</v>
+        <v>-0</v>
       </c>
       <c r="K36" t="n">
-        <v>327.77</v>
+        <v>250.53</v>
       </c>
       <c r="L36" t="n">
-        <v>181.8</v>
+        <v>-251.01</v>
       </c>
       <c r="M36" t="n">
-        <v>-252.55</v>
+        <v>-237.49</v>
       </c>
       <c r="N36" t="n">
-        <v>61.62</v>
+        <v>26.06</v>
       </c>
       <c r="O36" t="n">
         <v>-0</v>
@@ -2298,52 +2298,52 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>3270</t>
+          <t>4900</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Aarberg</t>
+          <t>Langenthal</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="D37" t="n">
-        <v>791.75</v>
+        <v>-70.77</v>
       </c>
       <c r="E37" t="n">
-        <v>531.97</v>
+        <v>33.06</v>
       </c>
       <c r="F37" t="n">
-        <v>-379.6</v>
+        <v>136.11</v>
       </c>
       <c r="G37" t="n">
-        <v>234.25</v>
+        <v>-93.63</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>344.24</v>
       </c>
       <c r="I37" t="n">
-        <v>164.45</v>
+        <v>-39.78</v>
       </c>
       <c r="J37" t="n">
-        <v>0</v>
+        <v>288.97</v>
       </c>
       <c r="K37" t="n">
-        <v>475.69</v>
+        <v>53.77</v>
       </c>
       <c r="L37" t="n">
-        <v>164.45</v>
+        <v>31.59</v>
       </c>
       <c r="M37" t="n">
-        <v>164.45</v>
+        <v>-26.52</v>
       </c>
       <c r="N37" t="n">
-        <v>164.45</v>
+        <v>13.54</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>33.17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in homegate scraper
</commit_message>
<xml_diff>
--- a/Data/results/results_supplementary_question.xlsx
+++ b/Data/results/results_supplementary_question.xlsx
@@ -513,211 +513,211 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2502</t>
+          <t>3012</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>200</v>
+        <v>58</v>
       </c>
       <c r="D2" t="n">
-        <v>140.97</v>
+        <v>165.82</v>
       </c>
       <c r="E2" t="n">
-        <v>-80.87</v>
+        <v>150.2</v>
       </c>
       <c r="F2" t="n">
-        <v>110.95</v>
+        <v>-39.57</v>
       </c>
       <c r="G2" t="n">
-        <v>73.77</v>
+        <v>26.88</v>
       </c>
       <c r="H2" t="n">
-        <v>212.16</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
-        <v>304.91</v>
+        <v>363.75</v>
       </c>
       <c r="J2" t="n">
-        <v>-41.03</v>
+        <v>581.58</v>
       </c>
       <c r="K2" t="n">
-        <v>121.69</v>
+        <v>229.38</v>
       </c>
       <c r="L2" t="n">
-        <v>-73.78</v>
+        <v>232.29</v>
       </c>
       <c r="M2" t="n">
-        <v>66.14</v>
+        <v>-68.38</v>
       </c>
       <c r="N2" t="n">
-        <v>-85.2</v>
+        <v>-22.6</v>
       </c>
       <c r="O2" t="n">
-        <v>-370.56</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>4912</t>
+          <t>3360</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Aarwangen</t>
+          <t>Herzogenbuchsee</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="D3" t="n">
-        <v>71.78</v>
+        <v>17.23</v>
       </c>
       <c r="E3" t="n">
-        <v>280.38</v>
+        <v>42.79</v>
       </c>
       <c r="F3" t="n">
-        <v>354.29</v>
+        <v>180.84</v>
       </c>
       <c r="G3" t="n">
-        <v>-125.02</v>
+        <v>-84.84</v>
       </c>
       <c r="H3" t="n">
-        <v>513.88</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>393.41</v>
+        <v>33.96</v>
       </c>
       <c r="J3" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>-18.33</v>
+        <v>78.56999999999999</v>
       </c>
       <c r="L3" t="n">
-        <v>-98</v>
+        <v>82.8</v>
       </c>
       <c r="M3" t="n">
-        <v>-8.74</v>
+        <v>62.8</v>
       </c>
       <c r="N3" t="n">
-        <v>-40.79</v>
+        <v>87.58</v>
       </c>
       <c r="O3" t="n">
-        <v>-0</v>
+        <v>245.97</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3014</t>
+          <t>4900</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Langenthal</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="D4" t="n">
-        <v>122.62</v>
+        <v>-70.77</v>
       </c>
       <c r="E4" t="n">
-        <v>-17.98</v>
+        <v>33.06</v>
       </c>
       <c r="F4" t="n">
-        <v>98.73</v>
+        <v>136.11</v>
       </c>
       <c r="G4" t="n">
-        <v>-180.25</v>
+        <v>-93.63</v>
       </c>
       <c r="H4" t="n">
-        <v>-0</v>
+        <v>344.24</v>
       </c>
       <c r="I4" t="n">
-        <v>932.66</v>
+        <v>-39.78</v>
       </c>
       <c r="J4" t="n">
-        <v>427.22</v>
+        <v>288.97</v>
       </c>
       <c r="K4" t="n">
-        <v>285.62</v>
+        <v>53.77</v>
       </c>
       <c r="L4" t="n">
-        <v>61.28</v>
+        <v>31.59</v>
       </c>
       <c r="M4" t="n">
-        <v>0.46</v>
+        <v>-26.52</v>
       </c>
       <c r="N4" t="n">
-        <v>-169.01</v>
+        <v>13.54</v>
       </c>
       <c r="O4" t="n">
-        <v>-128.79</v>
+        <v>33.17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3400</t>
+          <t>3008</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Burgdorf</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D5" t="n">
-        <v>-16.99</v>
+        <v>-437.15</v>
       </c>
       <c r="E5" t="n">
-        <v>126.14</v>
+        <v>393.76</v>
       </c>
       <c r="F5" t="n">
-        <v>57</v>
+        <v>-9.85</v>
       </c>
       <c r="G5" t="n">
-        <v>138.78</v>
+        <v>-90.37</v>
       </c>
       <c r="H5" t="n">
-        <v>206.61</v>
+        <v>352.94</v>
       </c>
       <c r="I5" t="n">
-        <v>-0</v>
+        <v>-89.97</v>
       </c>
       <c r="J5" t="n">
-        <v>246.1</v>
+        <v>205.93</v>
       </c>
       <c r="K5" t="n">
-        <v>223.49</v>
+        <v>75.23</v>
       </c>
       <c r="L5" t="n">
-        <v>146.57</v>
+        <v>-123.67</v>
       </c>
       <c r="M5" t="n">
-        <v>-285.68</v>
+        <v>-38.08</v>
       </c>
       <c r="N5" t="n">
-        <v>-4.57</v>
+        <v>-160.54</v>
       </c>
       <c r="O5" t="n">
-        <v>-3.99</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3008</t>
+          <t>3007</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -726,40 +726,40 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="D6" t="n">
-        <v>-437.15</v>
+        <v>-38.69</v>
       </c>
       <c r="E6" t="n">
-        <v>393.76</v>
+        <v>-5.92</v>
       </c>
       <c r="F6" t="n">
-        <v>-9.85</v>
+        <v>89.33</v>
       </c>
       <c r="G6" t="n">
-        <v>-90.37</v>
+        <v>53.71</v>
       </c>
       <c r="H6" t="n">
-        <v>352.94</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>-89.97</v>
+        <v>-73.17</v>
       </c>
       <c r="J6" t="n">
-        <v>205.93</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>75.23</v>
+        <v>80.76000000000001</v>
       </c>
       <c r="L6" t="n">
-        <v>-123.67</v>
+        <v>95.14</v>
       </c>
       <c r="M6" t="n">
-        <v>-38.08</v>
+        <v>-98.7</v>
       </c>
       <c r="N6" t="n">
-        <v>-160.54</v>
+        <v>-71.63</v>
       </c>
       <c r="O6" t="n">
         <v>0</v>
@@ -768,211 +768,211 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>3322</t>
+          <t>3302</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Urtenen-Schönbühl</t>
+          <t>Moosseedorf</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="n">
-        <v>-72.22</v>
+        <v>-46.21</v>
       </c>
       <c r="E7" t="n">
-        <v>114.24</v>
+        <v>114.91</v>
       </c>
       <c r="F7" t="n">
-        <v>24.27</v>
+        <v>178.14</v>
       </c>
       <c r="G7" t="n">
-        <v>-119.38</v>
+        <v>-356.93</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>-358.43</v>
       </c>
       <c r="I7" t="n">
-        <v>28.17</v>
+        <v>-0</v>
       </c>
       <c r="J7" t="n">
-        <v>53.19</v>
+        <v>279.22</v>
       </c>
       <c r="K7" t="n">
-        <v>-25.73</v>
+        <v>-10.83</v>
       </c>
       <c r="L7" t="n">
-        <v>85.84</v>
+        <v>-73.12</v>
       </c>
       <c r="M7" t="n">
-        <v>-152.09</v>
+        <v>128.33</v>
       </c>
       <c r="N7" t="n">
-        <v>60.13</v>
+        <v>53.29</v>
       </c>
       <c r="O7" t="n">
-        <v>52.04</v>
+        <v>-341.09</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>3414</t>
+          <t>3006</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Oberburg</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D8" t="n">
-        <v>15.37</v>
+        <v>160.21</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-22.52</v>
       </c>
       <c r="F8" t="n">
-        <v>233.14</v>
+        <v>561.87</v>
       </c>
       <c r="G8" t="n">
-        <v>284.46</v>
+        <v>490.92</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I8" t="n">
-        <v>-527.28</v>
+        <v>-0</v>
       </c>
       <c r="J8" t="n">
-        <v>349.82</v>
+        <v>-0</v>
       </c>
       <c r="K8" t="n">
-        <v>-527.28</v>
+        <v>629.9400000000001</v>
       </c>
       <c r="L8" t="n">
-        <v>-590.77</v>
+        <v>-352.17</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>483.45</v>
       </c>
       <c r="N8" t="n">
-        <v>353.43</v>
+        <v>-58.15</v>
       </c>
       <c r="O8" t="n">
-        <v>-590.77</v>
+        <v>-658.08</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>3600</t>
+          <t>4950</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Thun</t>
+          <t>Huttwil</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="D9" t="n">
-        <v>207.02</v>
+        <v>67.13</v>
       </c>
       <c r="E9" t="n">
-        <v>252.93</v>
+        <v>32.17</v>
       </c>
       <c r="F9" t="n">
-        <v>154.12</v>
+        <v>273.14</v>
       </c>
       <c r="G9" t="n">
-        <v>-202.6</v>
+        <v>-61.28</v>
       </c>
       <c r="H9" t="n">
-        <v>205.69</v>
+        <v>-0</v>
       </c>
       <c r="I9" t="n">
-        <v>-75.93000000000001</v>
+        <v>615.97</v>
       </c>
       <c r="J9" t="n">
-        <v>424.62</v>
+        <v>-0</v>
       </c>
       <c r="K9" t="n">
-        <v>159.97</v>
+        <v>388.76</v>
       </c>
       <c r="L9" t="n">
-        <v>399.38</v>
+        <v>275.64</v>
       </c>
       <c r="M9" t="n">
-        <v>-36.73</v>
+        <v>-40.09</v>
       </c>
       <c r="N9" t="n">
-        <v>69.09999999999999</v>
+        <v>-104.11</v>
       </c>
       <c r="O9" t="n">
-        <v>-309.26</v>
+        <v>13.91</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>3098</t>
+          <t>3063</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Köniz</t>
+          <t>Ittigen</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D10" t="n">
-        <v>-79.42</v>
+        <v>37.39</v>
       </c>
       <c r="E10" t="n">
-        <v>67.02</v>
+        <v>431.11</v>
       </c>
       <c r="F10" t="n">
-        <v>49.57</v>
+        <v>-186.35</v>
       </c>
       <c r="G10" t="n">
-        <v>-33.85</v>
+        <v>698.52</v>
       </c>
       <c r="H10" t="n">
-        <v>252.54</v>
+        <v>334.87</v>
       </c>
       <c r="I10" t="n">
-        <v>483.86</v>
+        <v>276.35</v>
       </c>
       <c r="J10" t="n">
-        <v>-0</v>
+        <v>104.12</v>
       </c>
       <c r="K10" t="n">
-        <v>314.85</v>
+        <v>165.96</v>
       </c>
       <c r="L10" t="n">
-        <v>-16.51</v>
+        <v>354.2</v>
       </c>
       <c r="M10" t="n">
-        <v>-17.51</v>
+        <v>-186.29</v>
       </c>
       <c r="N10" t="n">
-        <v>-38.6</v>
+        <v>-130.26</v>
       </c>
       <c r="O10" t="n">
-        <v>155.63</v>
+        <v>-13.12</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>3006</t>
+          <t>3018</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -981,457 +981,457 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D11" t="n">
-        <v>160.21</v>
+        <v>-196.57</v>
       </c>
       <c r="E11" t="n">
-        <v>-22.52</v>
+        <v>-140.72</v>
       </c>
       <c r="F11" t="n">
-        <v>561.87</v>
+        <v>42.27</v>
       </c>
       <c r="G11" t="n">
-        <v>490.92</v>
+        <v>119.98</v>
       </c>
       <c r="H11" t="n">
-        <v>-0</v>
+        <v>92.04000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>-0</v>
+        <v>102.11</v>
       </c>
       <c r="J11" t="n">
-        <v>-0</v>
+        <v>92.48999999999999</v>
       </c>
       <c r="K11" t="n">
-        <v>629.9400000000001</v>
+        <v>71.45</v>
       </c>
       <c r="L11" t="n">
-        <v>-352.17</v>
+        <v>35.82</v>
       </c>
       <c r="M11" t="n">
-        <v>483.45</v>
+        <v>-99.56</v>
       </c>
       <c r="N11" t="n">
-        <v>-58.15</v>
+        <v>-47.17</v>
       </c>
       <c r="O11" t="n">
-        <v>-658.08</v>
+        <v>-355.07</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3013</t>
+          <t>3072</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Ostermundigen</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="D12" t="n">
-        <v>-66.02</v>
+        <v>-149.15</v>
       </c>
       <c r="E12" t="n">
-        <v>-81.20999999999999</v>
+        <v>9.59</v>
       </c>
       <c r="F12" t="n">
-        <v>-84.18000000000001</v>
+        <v>86.14</v>
       </c>
       <c r="G12" t="n">
-        <v>228.05</v>
+        <v>-60.65</v>
       </c>
       <c r="H12" t="n">
-        <v>109.6</v>
+        <v>-273.53</v>
       </c>
       <c r="I12" t="n">
-        <v>-0</v>
+        <v>75.65000000000001</v>
       </c>
       <c r="J12" t="n">
-        <v>-102.41</v>
+        <v>433.65</v>
       </c>
       <c r="K12" t="n">
-        <v>327.77</v>
+        <v>89.5</v>
       </c>
       <c r="L12" t="n">
-        <v>181.8</v>
+        <v>39.7</v>
       </c>
       <c r="M12" t="n">
-        <v>-252.55</v>
+        <v>-128.77</v>
       </c>
       <c r="N12" t="n">
-        <v>61.62</v>
+        <v>45.48</v>
       </c>
       <c r="O12" t="n">
-        <v>-0</v>
+        <v>-61.79</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3097</t>
+          <t>3052</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Liebefeld</t>
+          <t>Zollikofen</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D13" t="n">
-        <v>4.83</v>
+        <v>73.94</v>
       </c>
       <c r="E13" t="n">
-        <v>317.67</v>
+        <v>45.36</v>
       </c>
       <c r="F13" t="n">
-        <v>-53.57</v>
+        <v>347.56</v>
       </c>
       <c r="G13" t="n">
-        <v>268.25</v>
+        <v>157.68</v>
       </c>
       <c r="H13" t="n">
-        <v>-0</v>
+        <v>382.34</v>
       </c>
       <c r="I13" t="n">
-        <v>-0</v>
+        <v>488.02</v>
       </c>
       <c r="J13" t="n">
-        <v>-0</v>
+        <v>457.62</v>
       </c>
       <c r="K13" t="n">
-        <v>165.67</v>
+        <v>456.47</v>
       </c>
       <c r="L13" t="n">
-        <v>293.8</v>
+        <v>135.73</v>
       </c>
       <c r="M13" t="n">
-        <v>-171.75</v>
+        <v>39.84</v>
       </c>
       <c r="N13" t="n">
-        <v>-185.21</v>
+        <v>-228.55</v>
       </c>
       <c r="O13" t="n">
-        <v>-0</v>
+        <v>-59.51</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>2560</t>
+          <t>3098</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Nidau</t>
+          <t>Köniz</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="D14" t="n">
-        <v>17.85</v>
+        <v>-79.42</v>
       </c>
       <c r="E14" t="n">
-        <v>-18.28</v>
+        <v>67.02</v>
       </c>
       <c r="F14" t="n">
-        <v>5.66</v>
+        <v>49.57</v>
       </c>
       <c r="G14" t="n">
-        <v>-8.58</v>
+        <v>-33.85</v>
       </c>
       <c r="H14" t="n">
-        <v>204.49</v>
+        <v>252.54</v>
       </c>
       <c r="I14" t="n">
-        <v>-232.04</v>
+        <v>483.86</v>
       </c>
       <c r="J14" t="n">
-        <v>12.96</v>
+        <v>-0</v>
       </c>
       <c r="K14" t="n">
-        <v>337.86</v>
+        <v>314.85</v>
       </c>
       <c r="L14" t="n">
-        <v>70.78</v>
+        <v>-16.51</v>
       </c>
       <c r="M14" t="n">
-        <v>-102.03</v>
+        <v>-17.51</v>
       </c>
       <c r="N14" t="n">
-        <v>-78.64</v>
+        <v>-38.6</v>
       </c>
       <c r="O14" t="n">
-        <v>-0</v>
+        <v>155.63</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3250</t>
+          <t>4912</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lyss</t>
+          <t>Aarwangen</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D15" t="n">
-        <v>211.29</v>
+        <v>71.78</v>
       </c>
       <c r="E15" t="n">
-        <v>-88.04000000000001</v>
+        <v>280.38</v>
       </c>
       <c r="F15" t="n">
-        <v>78.73</v>
+        <v>354.29</v>
       </c>
       <c r="G15" t="n">
-        <v>50.71</v>
+        <v>-125.02</v>
       </c>
       <c r="H15" t="n">
-        <v>-16.53</v>
+        <v>513.88</v>
       </c>
       <c r="I15" t="n">
-        <v>123.09</v>
+        <v>393.41</v>
       </c>
       <c r="J15" t="n">
-        <v>61.1</v>
+        <v>-0</v>
       </c>
       <c r="K15" t="n">
-        <v>325.03</v>
+        <v>-18.33</v>
       </c>
       <c r="L15" t="n">
-        <v>49.2</v>
+        <v>-98</v>
       </c>
       <c r="M15" t="n">
-        <v>11.76</v>
+        <v>-8.74</v>
       </c>
       <c r="N15" t="n">
-        <v>108.48</v>
+        <v>-40.79</v>
       </c>
       <c r="O15" t="n">
-        <v>70.54000000000001</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>4950</t>
+          <t>3014</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Huttwil</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="D16" t="n">
-        <v>67.13</v>
+        <v>122.62</v>
       </c>
       <c r="E16" t="n">
-        <v>32.17</v>
+        <v>-17.98</v>
       </c>
       <c r="F16" t="n">
-        <v>273.14</v>
+        <v>98.73</v>
       </c>
       <c r="G16" t="n">
-        <v>-61.28</v>
+        <v>-180.25</v>
       </c>
       <c r="H16" t="n">
         <v>-0</v>
       </c>
       <c r="I16" t="n">
-        <v>615.97</v>
+        <v>932.66</v>
       </c>
       <c r="J16" t="n">
-        <v>-0</v>
+        <v>427.22</v>
       </c>
       <c r="K16" t="n">
-        <v>388.76</v>
+        <v>285.62</v>
       </c>
       <c r="L16" t="n">
-        <v>275.64</v>
+        <v>61.28</v>
       </c>
       <c r="M16" t="n">
-        <v>-40.09</v>
+        <v>0.46</v>
       </c>
       <c r="N16" t="n">
-        <v>-104.11</v>
+        <v>-169.01</v>
       </c>
       <c r="O16" t="n">
-        <v>13.91</v>
+        <v>-128.79</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>2503</t>
+          <t>3322</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Urtenen-Schönbühl</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>170</v>
+        <v>24</v>
       </c>
       <c r="D17" t="n">
-        <v>45.56</v>
+        <v>-72.22</v>
       </c>
       <c r="E17" t="n">
-        <v>34.85</v>
+        <v>114.24</v>
       </c>
       <c r="F17" t="n">
-        <v>82.02</v>
+        <v>24.27</v>
       </c>
       <c r="G17" t="n">
-        <v>-48.1</v>
+        <v>-119.38</v>
       </c>
       <c r="H17" t="n">
-        <v>211.98</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
-        <v>391.57</v>
+        <v>28.17</v>
       </c>
       <c r="J17" t="n">
-        <v>244.93</v>
+        <v>53.19</v>
       </c>
       <c r="K17" t="n">
-        <v>79.42</v>
+        <v>-25.73</v>
       </c>
       <c r="L17" t="n">
-        <v>-46.71</v>
+        <v>85.84</v>
       </c>
       <c r="M17" t="n">
-        <v>-2.64</v>
+        <v>-152.09</v>
       </c>
       <c r="N17" t="n">
-        <v>59.75</v>
+        <v>60.13</v>
       </c>
       <c r="O17" t="n">
-        <v>56.46</v>
+        <v>52.04</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>3052</t>
+          <t>2502</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Zollikofen</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>29</v>
+        <v>200</v>
       </c>
       <c r="D18" t="n">
-        <v>73.94</v>
+        <v>140.97</v>
       </c>
       <c r="E18" t="n">
-        <v>45.36</v>
+        <v>-80.87</v>
       </c>
       <c r="F18" t="n">
-        <v>347.56</v>
+        <v>110.95</v>
       </c>
       <c r="G18" t="n">
-        <v>157.68</v>
+        <v>73.77</v>
       </c>
       <c r="H18" t="n">
-        <v>382.34</v>
+        <v>212.16</v>
       </c>
       <c r="I18" t="n">
-        <v>488.02</v>
+        <v>304.91</v>
       </c>
       <c r="J18" t="n">
-        <v>457.62</v>
+        <v>-41.03</v>
       </c>
       <c r="K18" t="n">
-        <v>456.47</v>
+        <v>121.69</v>
       </c>
       <c r="L18" t="n">
-        <v>135.73</v>
+        <v>-73.78</v>
       </c>
       <c r="M18" t="n">
-        <v>39.84</v>
+        <v>66.14</v>
       </c>
       <c r="N18" t="n">
-        <v>-228.55</v>
+        <v>-85.2</v>
       </c>
       <c r="O18" t="n">
-        <v>-59.51</v>
+        <v>-370.56</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>3302</t>
+          <t>2560</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Moosseedorf</t>
+          <t>Nidau</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D19" t="n">
-        <v>-46.21</v>
+        <v>17.85</v>
       </c>
       <c r="E19" t="n">
-        <v>114.91</v>
+        <v>-18.28</v>
       </c>
       <c r="F19" t="n">
-        <v>178.14</v>
+        <v>5.66</v>
       </c>
       <c r="G19" t="n">
-        <v>-356.93</v>
+        <v>-8.58</v>
       </c>
       <c r="H19" t="n">
-        <v>-358.43</v>
+        <v>204.49</v>
       </c>
       <c r="I19" t="n">
-        <v>-0</v>
+        <v>-232.04</v>
       </c>
       <c r="J19" t="n">
-        <v>279.22</v>
+        <v>12.96</v>
       </c>
       <c r="K19" t="n">
-        <v>-10.83</v>
+        <v>337.86</v>
       </c>
       <c r="L19" t="n">
-        <v>-73.12</v>
+        <v>70.78</v>
       </c>
       <c r="M19" t="n">
-        <v>128.33</v>
+        <v>-102.03</v>
       </c>
       <c r="N19" t="n">
-        <v>53.29</v>
+        <v>-78.64</v>
       </c>
       <c r="O19" t="n">
-        <v>-341.09</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>3018</t>
+          <t>3011</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -1440,91 +1440,91 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D20" t="n">
-        <v>-196.57</v>
+        <v>-22.4</v>
       </c>
       <c r="E20" t="n">
-        <v>-140.72</v>
+        <v>207.57</v>
       </c>
       <c r="F20" t="n">
-        <v>42.27</v>
+        <v>280.52</v>
       </c>
       <c r="G20" t="n">
-        <v>119.98</v>
+        <v>222.39</v>
       </c>
       <c r="H20" t="n">
-        <v>92.04000000000001</v>
+        <v>-0</v>
       </c>
       <c r="I20" t="n">
-        <v>102.11</v>
+        <v>-181.31</v>
       </c>
       <c r="J20" t="n">
-        <v>92.48999999999999</v>
+        <v>-361.86</v>
       </c>
       <c r="K20" t="n">
-        <v>71.45</v>
+        <v>86.22</v>
       </c>
       <c r="L20" t="n">
-        <v>35.82</v>
+        <v>-17.78</v>
       </c>
       <c r="M20" t="n">
-        <v>-99.56</v>
+        <v>2.18</v>
       </c>
       <c r="N20" t="n">
-        <v>-47.17</v>
+        <v>15.83</v>
       </c>
       <c r="O20" t="n">
-        <v>-355.07</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>3270</t>
+          <t>3027</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Aarberg</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D21" t="n">
-        <v>791.75</v>
+        <v>220.42</v>
       </c>
       <c r="E21" t="n">
-        <v>531.97</v>
+        <v>284.87</v>
       </c>
       <c r="F21" t="n">
-        <v>-379.6</v>
+        <v>195.56</v>
       </c>
       <c r="G21" t="n">
-        <v>234.25</v>
+        <v>274.62</v>
       </c>
       <c r="H21" t="n">
-        <v>0</v>
+        <v>293.3</v>
       </c>
       <c r="I21" t="n">
-        <v>164.45</v>
+        <v>286.67</v>
       </c>
       <c r="J21" t="n">
-        <v>0</v>
+        <v>567.71</v>
       </c>
       <c r="K21" t="n">
-        <v>475.69</v>
+        <v>155.65</v>
       </c>
       <c r="L21" t="n">
-        <v>164.45</v>
+        <v>-416.05</v>
       </c>
       <c r="M21" t="n">
-        <v>164.45</v>
+        <v>-153.66</v>
       </c>
       <c r="N21" t="n">
-        <v>164.45</v>
+        <v>78.76000000000001</v>
       </c>
       <c r="O21" t="n">
         <v>0</v>
@@ -1533,694 +1533,694 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4914</t>
+          <t>3013</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Roggwil BE</t>
+          <t>Bern</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="D22" t="n">
-        <v>-65.79000000000001</v>
+        <v>-66.02</v>
       </c>
       <c r="E22" t="n">
-        <v>134.94</v>
+        <v>-81.20999999999999</v>
       </c>
       <c r="F22" t="n">
-        <v>-60.78</v>
+        <v>-84.18000000000001</v>
       </c>
       <c r="G22" t="n">
-        <v>103</v>
+        <v>228.05</v>
       </c>
       <c r="H22" t="n">
-        <v>-83.68000000000001</v>
+        <v>109.6</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="J22" t="n">
-        <v>73.14</v>
+        <v>-102.41</v>
       </c>
       <c r="K22" t="n">
-        <v>-95.22</v>
+        <v>327.77</v>
       </c>
       <c r="L22" t="n">
-        <v>-26.73</v>
+        <v>181.8</v>
       </c>
       <c r="M22" t="n">
-        <v>0</v>
+        <v>-252.55</v>
       </c>
       <c r="N22" t="n">
-        <v>-1.22</v>
+        <v>61.62</v>
       </c>
       <c r="O22" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>4922</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Bützberg</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D23" t="n">
-        <v>-46.54</v>
+        <v>-27.36</v>
       </c>
       <c r="E23" t="n">
-        <v>52.29</v>
+        <v>161.33</v>
       </c>
       <c r="F23" t="n">
-        <v>158.67</v>
+        <v>412.9</v>
       </c>
       <c r="G23" t="n">
-        <v>-100</v>
+        <v>-266.33</v>
       </c>
       <c r="H23" t="n">
-        <v>-0</v>
+        <v>108.88</v>
       </c>
       <c r="I23" t="n">
-        <v>54.94</v>
+        <v>-0</v>
       </c>
       <c r="J23" t="n">
         <v>-0</v>
       </c>
       <c r="K23" t="n">
-        <v>155.38</v>
+        <v>306.15</v>
       </c>
       <c r="L23" t="n">
-        <v>-0</v>
+        <v>196.01</v>
       </c>
       <c r="M23" t="n">
-        <v>-184.61</v>
+        <v>109.56</v>
       </c>
       <c r="N23" t="n">
-        <v>-16.47</v>
+        <v>237.57</v>
       </c>
       <c r="O23" t="n">
-        <v>-0</v>
+        <v>165.34</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>3012</t>
+          <t>2555</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Brügg BE</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D24" t="n">
-        <v>165.82</v>
+        <v>41.52</v>
       </c>
       <c r="E24" t="n">
-        <v>150.2</v>
+        <v>-44.19</v>
       </c>
       <c r="F24" t="n">
-        <v>-39.57</v>
+        <v>6.89</v>
       </c>
       <c r="G24" t="n">
-        <v>26.88</v>
+        <v>4.3</v>
       </c>
       <c r="H24" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="I24" t="n">
-        <v>363.75</v>
+        <v>-75.98999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>581.58</v>
+        <v>222.7</v>
       </c>
       <c r="K24" t="n">
-        <v>229.38</v>
+        <v>222.7</v>
       </c>
       <c r="L24" t="n">
-        <v>232.29</v>
+        <v>10.49</v>
       </c>
       <c r="M24" t="n">
-        <v>-68.38</v>
+        <v>-0</v>
       </c>
       <c r="N24" t="n">
-        <v>-22.6</v>
+        <v>-22.58</v>
       </c>
       <c r="O24" t="n">
-        <v>0</v>
+        <v>-73.26000000000001</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>3084</t>
+          <t>2504</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Wabern</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>24</v>
+        <v>76</v>
       </c>
       <c r="D25" t="n">
-        <v>6.43</v>
+        <v>-15.72</v>
       </c>
       <c r="E25" t="n">
-        <v>-11.5</v>
+        <v>55.74</v>
       </c>
       <c r="F25" t="n">
-        <v>-219.67</v>
+        <v>-54.3</v>
       </c>
       <c r="G25" t="n">
-        <v>-196.73</v>
+        <v>-97.48999999999999</v>
       </c>
       <c r="H25" t="n">
-        <v>90.03</v>
+        <v>-0</v>
       </c>
       <c r="I25" t="n">
-        <v>952.75</v>
+        <v>37.13</v>
       </c>
       <c r="J25" t="n">
-        <v>-0</v>
+        <v>-44.7</v>
       </c>
       <c r="K25" t="n">
-        <v>104.41</v>
+        <v>272.76</v>
       </c>
       <c r="L25" t="n">
-        <v>28.27</v>
+        <v>42.35</v>
       </c>
       <c r="M25" t="n">
-        <v>128.82</v>
+        <v>-47.58</v>
       </c>
       <c r="N25" t="n">
-        <v>292.5</v>
+        <v>-96.93000000000001</v>
       </c>
       <c r="O25" t="n">
-        <v>-75.93000000000001</v>
+        <v>-98.81</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>3072</t>
+          <t>3110</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Ostermundigen</t>
+          <t>Münsingen</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="D26" t="n">
-        <v>-149.15</v>
+        <v>26.34</v>
       </c>
       <c r="E26" t="n">
-        <v>9.59</v>
+        <v>-73.05</v>
       </c>
       <c r="F26" t="n">
-        <v>86.14</v>
+        <v>121.32</v>
       </c>
       <c r="G26" t="n">
-        <v>-60.65</v>
+        <v>61.99</v>
       </c>
       <c r="H26" t="n">
-        <v>-273.53</v>
+        <v>-0</v>
       </c>
       <c r="I26" t="n">
-        <v>75.65000000000001</v>
+        <v>-0</v>
       </c>
       <c r="J26" t="n">
-        <v>433.65</v>
+        <v>-0</v>
       </c>
       <c r="K26" t="n">
-        <v>89.5</v>
+        <v>250.53</v>
       </c>
       <c r="L26" t="n">
-        <v>39.7</v>
+        <v>-251.01</v>
       </c>
       <c r="M26" t="n">
-        <v>-128.77</v>
+        <v>-237.49</v>
       </c>
       <c r="N26" t="n">
-        <v>45.48</v>
+        <v>26.06</v>
       </c>
       <c r="O26" t="n">
-        <v>-61.79</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2555</t>
+          <t>3084</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Brügg BE</t>
+          <t>Wabern</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="D27" t="n">
-        <v>41.52</v>
+        <v>6.43</v>
       </c>
       <c r="E27" t="n">
-        <v>-44.19</v>
+        <v>-11.5</v>
       </c>
       <c r="F27" t="n">
-        <v>6.89</v>
+        <v>-219.67</v>
       </c>
       <c r="G27" t="n">
-        <v>4.3</v>
+        <v>-196.73</v>
       </c>
       <c r="H27" t="n">
-        <v>-0</v>
+        <v>90.03</v>
       </c>
       <c r="I27" t="n">
-        <v>-75.98999999999999</v>
+        <v>952.75</v>
       </c>
       <c r="J27" t="n">
-        <v>222.7</v>
+        <v>-0</v>
       </c>
       <c r="K27" t="n">
-        <v>222.7</v>
+        <v>104.41</v>
       </c>
       <c r="L27" t="n">
-        <v>10.49</v>
+        <v>28.27</v>
       </c>
       <c r="M27" t="n">
-        <v>-0</v>
+        <v>128.82</v>
       </c>
       <c r="N27" t="n">
-        <v>-22.58</v>
+        <v>292.5</v>
       </c>
       <c r="O27" t="n">
-        <v>-73.26000000000001</v>
+        <v>-75.93000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>3007</t>
+          <t>3600</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Thun</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="D28" t="n">
-        <v>-38.69</v>
+        <v>207.02</v>
       </c>
       <c r="E28" t="n">
-        <v>-5.92</v>
+        <v>252.93</v>
       </c>
       <c r="F28" t="n">
-        <v>89.33</v>
+        <v>154.12</v>
       </c>
       <c r="G28" t="n">
-        <v>53.71</v>
+        <v>-202.6</v>
       </c>
       <c r="H28" t="n">
-        <v>0</v>
+        <v>205.69</v>
       </c>
       <c r="I28" t="n">
-        <v>-73.17</v>
+        <v>-75.93000000000001</v>
       </c>
       <c r="J28" t="n">
-        <v>0</v>
+        <v>424.62</v>
       </c>
       <c r="K28" t="n">
-        <v>80.76000000000001</v>
+        <v>159.97</v>
       </c>
       <c r="L28" t="n">
-        <v>95.14</v>
+        <v>399.38</v>
       </c>
       <c r="M28" t="n">
-        <v>-98.7</v>
+        <v>-36.73</v>
       </c>
       <c r="N28" t="n">
-        <v>-71.63</v>
+        <v>69.09999999999999</v>
       </c>
       <c r="O28" t="n">
-        <v>0</v>
+        <v>-309.26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>3063</t>
+          <t>3414</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Ittigen</t>
+          <t>Oberburg</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D29" t="n">
-        <v>37.39</v>
+        <v>15.37</v>
       </c>
       <c r="E29" t="n">
-        <v>431.11</v>
+        <v>0</v>
       </c>
       <c r="F29" t="n">
-        <v>-186.35</v>
+        <v>233.14</v>
       </c>
       <c r="G29" t="n">
-        <v>698.52</v>
+        <v>284.46</v>
       </c>
       <c r="H29" t="n">
-        <v>334.87</v>
+        <v>0</v>
       </c>
       <c r="I29" t="n">
-        <v>276.35</v>
+        <v>-527.28</v>
       </c>
       <c r="J29" t="n">
-        <v>104.12</v>
+        <v>349.82</v>
       </c>
       <c r="K29" t="n">
-        <v>165.96</v>
+        <v>-527.28</v>
       </c>
       <c r="L29" t="n">
-        <v>354.2</v>
+        <v>-590.77</v>
       </c>
       <c r="M29" t="n">
-        <v>-186.29</v>
+        <v>0</v>
       </c>
       <c r="N29" t="n">
-        <v>-130.26</v>
+        <v>353.43</v>
       </c>
       <c r="O29" t="n">
-        <v>-13.12</v>
+        <v>-590.77</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>3360</t>
+          <t>2503</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Herzogenbuchsee</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>40</v>
+        <v>170</v>
       </c>
       <c r="D30" t="n">
-        <v>17.23</v>
+        <v>45.56</v>
       </c>
       <c r="E30" t="n">
-        <v>42.79</v>
+        <v>34.85</v>
       </c>
       <c r="F30" t="n">
-        <v>180.84</v>
+        <v>82.02</v>
       </c>
       <c r="G30" t="n">
-        <v>-84.84</v>
+        <v>-48.1</v>
       </c>
       <c r="H30" t="n">
-        <v>0</v>
+        <v>211.98</v>
       </c>
       <c r="I30" t="n">
-        <v>33.96</v>
+        <v>391.57</v>
       </c>
       <c r="J30" t="n">
-        <v>0</v>
+        <v>244.93</v>
       </c>
       <c r="K30" t="n">
-        <v>78.56999999999999</v>
+        <v>79.42</v>
       </c>
       <c r="L30" t="n">
-        <v>82.8</v>
+        <v>-46.71</v>
       </c>
       <c r="M30" t="n">
-        <v>62.8</v>
+        <v>-2.64</v>
       </c>
       <c r="N30" t="n">
-        <v>87.58</v>
+        <v>59.75</v>
       </c>
       <c r="O30" t="n">
-        <v>245.97</v>
+        <v>56.46</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>3027</t>
+          <t>2500</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Biel/Bienne</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D31" t="n">
-        <v>220.42</v>
+        <v>-46.54</v>
       </c>
       <c r="E31" t="n">
-        <v>284.87</v>
+        <v>52.29</v>
       </c>
       <c r="F31" t="n">
-        <v>195.56</v>
+        <v>158.67</v>
       </c>
       <c r="G31" t="n">
-        <v>274.62</v>
+        <v>-100</v>
       </c>
       <c r="H31" t="n">
-        <v>293.3</v>
+        <v>-0</v>
       </c>
       <c r="I31" t="n">
-        <v>286.67</v>
+        <v>54.94</v>
       </c>
       <c r="J31" t="n">
-        <v>567.71</v>
+        <v>-0</v>
       </c>
       <c r="K31" t="n">
-        <v>155.65</v>
+        <v>155.38</v>
       </c>
       <c r="L31" t="n">
-        <v>-416.05</v>
+        <v>-0</v>
       </c>
       <c r="M31" t="n">
-        <v>-153.66</v>
+        <v>-184.61</v>
       </c>
       <c r="N31" t="n">
-        <v>78.76000000000001</v>
+        <v>-16.47</v>
       </c>
       <c r="O31" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>3073</t>
+          <t>3270</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gümligen</t>
+          <t>Aarberg</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D32" t="n">
-        <v>-88.77</v>
+        <v>791.75</v>
       </c>
       <c r="E32" t="n">
-        <v>126.5</v>
+        <v>531.97</v>
       </c>
       <c r="F32" t="n">
-        <v>41.54</v>
+        <v>-379.6</v>
       </c>
       <c r="G32" t="n">
-        <v>135</v>
+        <v>234.25</v>
       </c>
       <c r="H32" t="n">
-        <v>123.04</v>
+        <v>0</v>
       </c>
       <c r="I32" t="n">
-        <v>126.72</v>
+        <v>164.45</v>
       </c>
       <c r="J32" t="n">
-        <v>126.72</v>
+        <v>0</v>
       </c>
       <c r="K32" t="n">
-        <v>160.98</v>
+        <v>475.69</v>
       </c>
       <c r="L32" t="n">
-        <v>85.52</v>
+        <v>164.45</v>
       </c>
       <c r="M32" t="n">
-        <v>-187.81</v>
+        <v>164.45</v>
       </c>
       <c r="N32" t="n">
-        <v>102.04</v>
+        <v>164.45</v>
       </c>
       <c r="O32" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>3011</t>
+          <t>4914</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Bern</t>
+          <t>Roggwil BE</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D33" t="n">
-        <v>-22.4</v>
+        <v>-65.79000000000001</v>
       </c>
       <c r="E33" t="n">
-        <v>207.57</v>
+        <v>134.94</v>
       </c>
       <c r="F33" t="n">
-        <v>280.52</v>
+        <v>-60.78</v>
       </c>
       <c r="G33" t="n">
-        <v>222.39</v>
+        <v>103</v>
       </c>
       <c r="H33" t="n">
-        <v>-0</v>
+        <v>-83.68000000000001</v>
       </c>
       <c r="I33" t="n">
-        <v>-181.31</v>
+        <v>0</v>
       </c>
       <c r="J33" t="n">
-        <v>-361.86</v>
+        <v>73.14</v>
       </c>
       <c r="K33" t="n">
-        <v>86.22</v>
+        <v>-95.22</v>
       </c>
       <c r="L33" t="n">
-        <v>-17.78</v>
+        <v>-26.73</v>
       </c>
       <c r="M33" t="n">
-        <v>2.18</v>
+        <v>0</v>
       </c>
       <c r="N33" t="n">
-        <v>15.83</v>
+        <v>-1.22</v>
       </c>
       <c r="O33" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2504</t>
+          <t>3400</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Biel/Bienne</t>
+          <t>Burgdorf</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D34" t="n">
-        <v>-15.72</v>
+        <v>-16.99</v>
       </c>
       <c r="E34" t="n">
-        <v>55.74</v>
+        <v>126.14</v>
       </c>
       <c r="F34" t="n">
-        <v>-54.3</v>
+        <v>57</v>
       </c>
       <c r="G34" t="n">
-        <v>-97.48999999999999</v>
+        <v>138.78</v>
       </c>
       <c r="H34" t="n">
-        <v>-0</v>
+        <v>206.61</v>
       </c>
       <c r="I34" t="n">
-        <v>37.13</v>
+        <v>-0</v>
       </c>
       <c r="J34" t="n">
-        <v>-44.7</v>
+        <v>246.1</v>
       </c>
       <c r="K34" t="n">
-        <v>272.76</v>
+        <v>223.49</v>
       </c>
       <c r="L34" t="n">
-        <v>42.35</v>
+        <v>146.57</v>
       </c>
       <c r="M34" t="n">
-        <v>-47.58</v>
+        <v>-285.68</v>
       </c>
       <c r="N34" t="n">
-        <v>-96.93000000000001</v>
+        <v>-4.57</v>
       </c>
       <c r="O34" t="n">
-        <v>-98.81</v>
+        <v>-3.99</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4922</t>
+          <t>3097</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bützberg</t>
+          <t>Liebefeld</t>
         </is>
       </c>
       <c r="C35" t="n">
         <v>27</v>
       </c>
       <c r="D35" t="n">
-        <v>-27.36</v>
+        <v>4.83</v>
       </c>
       <c r="E35" t="n">
-        <v>161.33</v>
+        <v>317.67</v>
       </c>
       <c r="F35" t="n">
-        <v>412.9</v>
+        <v>-53.57</v>
       </c>
       <c r="G35" t="n">
-        <v>-266.33</v>
+        <v>268.25</v>
       </c>
       <c r="H35" t="n">
-        <v>108.88</v>
+        <v>-0</v>
       </c>
       <c r="I35" t="n">
         <v>-0</v>
@@ -2229,67 +2229,67 @@
         <v>-0</v>
       </c>
       <c r="K35" t="n">
-        <v>306.15</v>
+        <v>165.67</v>
       </c>
       <c r="L35" t="n">
-        <v>196.01</v>
+        <v>293.8</v>
       </c>
       <c r="M35" t="n">
-        <v>109.56</v>
+        <v>-171.75</v>
       </c>
       <c r="N35" t="n">
-        <v>237.57</v>
+        <v>-185.21</v>
       </c>
       <c r="O35" t="n">
-        <v>165.34</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>3110</t>
+          <t>3073</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Münsingen</t>
+          <t>Gümligen</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D36" t="n">
-        <v>26.34</v>
+        <v>-88.77</v>
       </c>
       <c r="E36" t="n">
-        <v>-73.05</v>
+        <v>126.5</v>
       </c>
       <c r="F36" t="n">
-        <v>121.32</v>
+        <v>41.54</v>
       </c>
       <c r="G36" t="n">
-        <v>61.99</v>
+        <v>135</v>
       </c>
       <c r="H36" t="n">
-        <v>-0</v>
+        <v>123.04</v>
       </c>
       <c r="I36" t="n">
-        <v>-0</v>
+        <v>126.72</v>
       </c>
       <c r="J36" t="n">
-        <v>-0</v>
+        <v>126.72</v>
       </c>
       <c r="K36" t="n">
-        <v>250.53</v>
+        <v>160.98</v>
       </c>
       <c r="L36" t="n">
-        <v>-251.01</v>
+        <v>85.52</v>
       </c>
       <c r="M36" t="n">
-        <v>-237.49</v>
+        <v>-187.81</v>
       </c>
       <c r="N36" t="n">
-        <v>26.06</v>
+        <v>102.04</v>
       </c>
       <c r="O36" t="n">
         <v>-0</v>
@@ -2298,52 +2298,52 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4900</t>
+          <t>3250</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Langenthal</t>
+          <t>Lyss</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>79</v>
+        <v>35</v>
       </c>
       <c r="D37" t="n">
-        <v>-70.77</v>
+        <v>211.29</v>
       </c>
       <c r="E37" t="n">
-        <v>33.06</v>
+        <v>-88.04000000000001</v>
       </c>
       <c r="F37" t="n">
-        <v>136.11</v>
+        <v>78.73</v>
       </c>
       <c r="G37" t="n">
-        <v>-93.63</v>
+        <v>50.71</v>
       </c>
       <c r="H37" t="n">
-        <v>344.24</v>
+        <v>-16.53</v>
       </c>
       <c r="I37" t="n">
-        <v>-39.78</v>
+        <v>123.09</v>
       </c>
       <c r="J37" t="n">
-        <v>288.97</v>
+        <v>61.1</v>
       </c>
       <c r="K37" t="n">
-        <v>53.77</v>
+        <v>325.03</v>
       </c>
       <c r="L37" t="n">
-        <v>31.59</v>
+        <v>49.2</v>
       </c>
       <c r="M37" t="n">
-        <v>-26.52</v>
+        <v>11.76</v>
       </c>
       <c r="N37" t="n">
-        <v>13.54</v>
+        <v>108.48</v>
       </c>
       <c r="O37" t="n">
-        <v>33.17</v>
+        <v>70.54000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>